<commit_message>
last update before vacay
</commit_message>
<xml_diff>
--- a/Duplicates.xlsx
+++ b/Duplicates.xlsx
@@ -8,14 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/93e7bf715ca369db/Dokument/GitHub/peptidomic_py/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="11_FFC65FC06B99E8E14C170BDA53AFAED66E066E0B" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F2E8372A-4DC1-4A6A-908C-8BED4C8A340C}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="11_FFC65FC06B99E8E14C170BDA53AFAED66E066E0B" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B3679031-B19A-468C-8835-455BB7E05E93}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -856,10 +866,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P81"/>
+  <dimension ref="A1:P82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" zoomScale="62" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4920,6 +4930,28 @@
         <v>131</v>
       </c>
     </row>
+    <row r="82" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="G82">
+        <f>COUNT(G2:G81)-COUNTIF(G2:G81,0)</f>
+        <v>25</v>
+      </c>
+      <c r="H82">
+        <f t="shared" ref="H82:K82" si="0">COUNT(H2:H81)-COUNTIF(H2:H81,0)</f>
+        <v>25</v>
+      </c>
+      <c r="I82">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="J82">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="K82">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>